<commit_message>
Korrektur Doku Anschlüsse Arduino
</commit_message>
<xml_diff>
--- a/doku/Anschlüsse Arduino.xlsx
+++ b/doku/Anschlüsse Arduino.xlsx
@@ -102,28 +102,28 @@
     <t xml:space="preserve">D 8</t>
   </si>
   <si>
+    <t xml:space="preserve">Treiber Schrittmotor Stunden-Achse Richtung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digitalausgang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Treiber Schrittmotor Stunden-Achse Einzelschritt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D 10</t>
+  </si>
+  <si>
     <t xml:space="preserve">Treiber Schrittmotor Deklinations-Achse Richtung</t>
   </si>
   <si>
-    <t xml:space="preserve">Digitalausgang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D 9</t>
+    <t xml:space="preserve">D 11</t>
   </si>
   <si>
     <t xml:space="preserve">Treiber Schrittmotor Deklinations-Achse Einzelschritt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treiber Schrittmotor Stunden-Achse Richtung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treiber Schrittmotor Stunden-Achse Einzelschritt</t>
   </si>
   <si>
     <t xml:space="preserve">D 30</t>
@@ -332,7 +332,7 @@
     <numFmt numFmtId="167" formatCode="#,##0.0&quot; m³&quot;"/>
     <numFmt numFmtId="168" formatCode="0"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -411,11 +411,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -463,7 +458,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -560,10 +555,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -585,20 +576,20 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="50.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="24.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="11.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="11.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="15.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="11.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="11.19"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2803,7 +2794,7 @@
       <c r="A14" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="16" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="17" t="s">
@@ -2831,7 +2822,7 @@
       <c r="A16" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="19" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="17" t="s">
@@ -3095,7 +3086,7 @@
       <c r="A37" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B37" s="24" t="s">
+      <c r="B37" s="16" t="s">
         <v>63</v>
       </c>
       <c r="C37" s="17" t="s">

</xml_diff>